<commit_message>
Modulo 1 y 2
</commit_message>
<xml_diff>
--- a/tests_cases/TPO - PE-16.xlsx
+++ b/tests_cases/TPO - PE-16.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Aplicaciones\Proyectos\TestingAplicaciones-MatrixTesters-TPO\tests_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B156E86-CC71-439C-8602-E14FCBA185FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70ADFE48-F878-4BE9-A2FA-13CDF7E2F431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="24270" windowHeight="11385" activeTab="2" xr2:uid="{DCE1F527-8622-40D5-806A-6A7E2BCE07A3}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="24270" windowHeight="11385" activeTab="2" xr2:uid="{DCE1F527-8622-40D5-806A-6A7E2BCE07A3}"/>
   </bookViews>
   <sheets>
     <sheet name="MT-01" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="98">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Expected Results</t>
   </si>
   <si>
-    <t>1.0</t>
-  </si>
-  <si>
     <t>Abrir la aplicación</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>Botón Registrar se habilita</t>
   </si>
   <si>
-    <t>1.4</t>
-  </si>
-  <si>
     <t>Denise Posklinski</t>
   </si>
   <si>
@@ -278,13 +272,73 @@
   </si>
   <si>
     <t>1.1</t>
+  </si>
+  <si>
+    <t>Executions</t>
+  </si>
+  <si>
+    <t>Regression 1</t>
+  </si>
+  <si>
+    <t>Regression 2</t>
+  </si>
+  <si>
+    <t>Regression 3</t>
+  </si>
+  <si>
+    <t>Regression 4</t>
+  </si>
+  <si>
+    <t>Tester:</t>
+  </si>
+  <si>
+    <t>Actual Results</t>
+  </si>
+  <si>
+    <t>Pass / Fail / Not executed / Suspended</t>
+  </si>
+  <si>
+    <t>As Expected</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Not executed</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Tester: Denise Posklinski</t>
+  </si>
+  <si>
+    <t>Clic en Sign in</t>
+  </si>
+  <si>
+    <t>Se abre página de ingreso</t>
+  </si>
+  <si>
+    <t>Clic en Register here</t>
+  </si>
+  <si>
+    <t>Se abre formulario de  registro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tester: </t>
+  </si>
+  <si>
+    <t>Validación de mail (No está en uso)</t>
+  </si>
+  <si>
+    <t>2.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,8 +403,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,8 +452,18 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -501,13 +601,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -569,6 +727,33 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -581,62 +766,64 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Celda de comprobación" xfId="4" builtinId="23"/>
+    <cellStyle name="Entrada" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{C558A088-66ED-4D97-B86E-4769E988BE41}"/>
     <cellStyle name="Note 2" xfId="2" xr:uid="{4BAC1941-5BF2-43E8-B9DC-8FEA0AFAB3F9}"/>
@@ -953,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3CCAC7-6C0E-44CD-ADA1-CF7A0722318C}">
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F2"/>
+    <sheetView topLeftCell="C18" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,46 +1168,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="D1" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="D2" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="33"/>
+      <c r="E3" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="40"/>
       <c r="G3" s="3"/>
       <c r="I3" s="3"/>
       <c r="K3" s="3"/>
@@ -1085,42 +1272,42 @@
       <c r="D7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="48"/>
     </row>
     <row r="8" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>1</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="17">
         <v>1</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="29"/>
+      <c r="E8" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="17">
         <v>2</v>
       </c>
-      <c r="E9" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="35"/>
+      <c r="E9" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="42"/>
     </row>
     <row r="10" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
@@ -1129,10 +1316,10 @@
       <c r="D10" s="17">
         <v>3</v>
       </c>
-      <c r="E10" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="35"/>
+      <c r="E10" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="42"/>
       <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1142,10 +1329,10 @@
       <c r="D11" s="17">
         <v>4</v>
       </c>
-      <c r="E11" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="35"/>
+      <c r="E11" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="42"/>
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1155,10 +1342,10 @@
       <c r="D12" s="17">
         <v>5</v>
       </c>
-      <c r="E12" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="35"/>
+      <c r="E12" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="42"/>
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1168,10 +1355,10 @@
       <c r="D13" s="17">
         <v>6</v>
       </c>
-      <c r="E13" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="35"/>
+      <c r="E13" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="42"/>
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1181,10 +1368,10 @@
       <c r="D14" s="17">
         <v>7</v>
       </c>
-      <c r="E14" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="35"/>
+      <c r="E14" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="42"/>
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1194,10 +1381,10 @@
       <c r="D15" s="17">
         <v>8</v>
       </c>
-      <c r="E15" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="35"/>
+      <c r="E15" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="42"/>
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1207,296 +1394,549 @@
       <c r="D16" s="17">
         <v>9</v>
       </c>
-      <c r="E16" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="35"/>
-    </row>
-    <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="42"/>
+    </row>
+    <row r="17" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="20"/>
       <c r="C17" s="10"/>
       <c r="D17" s="17">
         <v>10</v>
       </c>
-      <c r="E17" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="35"/>
-    </row>
-    <row r="18" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="42"/>
+    </row>
+    <row r="18" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
       <c r="C18" s="10"/>
       <c r="D18" s="17">
         <v>11</v>
       </c>
-      <c r="E18" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="29"/>
-    </row>
-    <row r="19" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="36"/>
+    </row>
+    <row r="19" spans="1:15" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+    <row r="20" spans="1:15" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="H20" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+    </row>
+    <row r="21" spans="1:15" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-    </row>
-    <row r="21" spans="1:6" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-    </row>
-    <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="18" t="s">
+      <c r="C21" s="45"/>
+      <c r="D21" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E21" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="38"/>
-    </row>
-    <row r="23" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="F21" s="45"/>
+      <c r="H21" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="O21" s="26"/>
+    </row>
+    <row r="22" spans="1:15" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="29"/>
+      <c r="J22" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="K22" s="29"/>
+      <c r="L22" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="M22" s="29"/>
+      <c r="N22" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="O22" s="29"/>
+    </row>
+    <row r="23" spans="1:15" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B23" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="28"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="38"/>
+      <c r="F23" s="39"/>
+      <c r="H23" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="K23" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="L23" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="M23" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="N23" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="O23" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>1</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="33"/>
       <c r="D24" s="30" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E24" s="31"/>
       <c r="F24" s="32"/>
-    </row>
-    <row r="25" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="24"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="25"/>
+    </row>
+    <row r="25" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>1</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="23"/>
-    </row>
-    <row r="26" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="32"/>
+      <c r="D25" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="32"/>
+      <c r="H25" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J25" s="24"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="25"/>
+    </row>
+    <row r="26" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>2</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="23"/>
-    </row>
-    <row r="27" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="32"/>
+      <c r="D26" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
+      <c r="H26" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J26" s="24"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="25"/>
+    </row>
+    <row r="27" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>3</v>
-      </c>
-      <c r="B27" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="33"/>
+      <c r="D27" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
+      <c r="H27" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" s="24"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="25"/>
+    </row>
+    <row r="28" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>6</v>
+      </c>
+      <c r="B28" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="21" t="s">
+      <c r="C28" s="33"/>
+      <c r="D28" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
+      <c r="H28" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J28" s="24"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="25"/>
+    </row>
+    <row r="29" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>7</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="33"/>
+      <c r="D29" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
+      <c r="H29" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J29" s="24"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="25"/>
+    </row>
+    <row r="30" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>8</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="33"/>
+      <c r="D30" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
+      <c r="H30" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I30" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J30" s="24"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="25"/>
+    </row>
+    <row r="31" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>9</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="33"/>
+      <c r="D31" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="31"/>
+      <c r="F31" s="32"/>
+      <c r="H31" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I31" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J31" s="24"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="25"/>
+    </row>
+    <row r="32" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>10</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="33"/>
+      <c r="D32" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="31"/>
+      <c r="F32" s="32"/>
+      <c r="H32" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I32" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J32" s="24"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="25"/>
+    </row>
+    <row r="33" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>11</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="33"/>
+      <c r="D33" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32"/>
+      <c r="H33" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I33" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J33" s="24"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="25"/>
+    </row>
+    <row r="34" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>12</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="33"/>
+      <c r="D34" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
+      <c r="H34" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I34" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J34" s="24"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="25"/>
+    </row>
+    <row r="35" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>13</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="33"/>
+      <c r="D35" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" s="31"/>
+      <c r="F35" s="32"/>
+      <c r="H35" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I35" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J35" s="24"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="25"/>
+    </row>
+    <row r="36" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>14</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="33"/>
+      <c r="D36" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="31"/>
+      <c r="F36" s="32"/>
+      <c r="H36" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I36" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J36" s="24"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="25"/>
+    </row>
+    <row r="37" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>15</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="33"/>
+      <c r="D37" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="31"/>
+      <c r="F37" s="32"/>
+      <c r="H37" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I37" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J37" s="24"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="25"/>
+    </row>
+    <row r="38" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>16</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="33"/>
+      <c r="D38" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="22"/>
-      <c r="F27" s="23"/>
-    </row>
-    <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>4</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="22"/>
-      <c r="F28" s="23"/>
-    </row>
-    <row r="29" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>5</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="23"/>
-    </row>
-    <row r="30" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
-        <v>6</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="22"/>
-      <c r="F30" s="23"/>
-    </row>
-    <row r="31" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
-        <v>7</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="22"/>
-      <c r="F31" s="23"/>
-    </row>
-    <row r="32" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
-        <v>8</v>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="22"/>
-      <c r="F32" s="23"/>
-    </row>
-    <row r="33" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>9</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="22"/>
-      <c r="F33" s="23"/>
-    </row>
-    <row r="34" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>10</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="22"/>
-      <c r="F34" s="23"/>
-    </row>
-    <row r="35" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>11</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="24"/>
-      <c r="D35" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="22"/>
-      <c r="F35" s="23"/>
-    </row>
-    <row r="36" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
-        <v>12</v>
-      </c>
-      <c r="B36" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="24"/>
-      <c r="D36" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" s="22"/>
-      <c r="F36" s="23"/>
-    </row>
-    <row r="37" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>13</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="24"/>
-      <c r="D37" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37" s="22"/>
-      <c r="F37" s="23"/>
-    </row>
-    <row r="38" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
-        <v>14</v>
-      </c>
-      <c r="B38" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="24"/>
-      <c r="D38" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E38" s="22"/>
-      <c r="F38" s="23"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="32"/>
+      <c r="H38" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I38" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J38" s="24"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="25"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="60">
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="D2:F2"/>
-    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E7:F7"/>
@@ -1518,20 +1958,21 @@
     <mergeCell ref="D31:F31"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B20:F21"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="B36:C36"/>
@@ -1542,6 +1983,15 @@
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="D37:F37"/>
     <mergeCell ref="D38:F38"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="H20:O20"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1550,10 +2000,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1891FC72-E65D-47E1-A5E8-C6F7D1AC5217}">
-  <dimension ref="A1:W22"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F2"/>
+    <sheetView topLeftCell="A16" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,46 +2030,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="D1" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="D2" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="33"/>
+      <c r="E3" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="40"/>
       <c r="G3" s="3"/>
       <c r="I3" s="3"/>
       <c r="K3" s="3"/>
@@ -1646,7 +2096,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1684,204 +2134,401 @@
       <c r="D7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="48"/>
     </row>
     <row r="8" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>1</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="16">
         <v>1</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="29"/>
+      <c r="E8" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="16">
         <v>2</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="29"/>
-    </row>
-    <row r="10" spans="1:23" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="10" spans="1:23" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:23" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-    </row>
-    <row r="12" spans="1:23" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-    </row>
-    <row r="13" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="B11" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="H11" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+    </row>
+    <row r="12" spans="1:23" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="18" t="s">
+      <c r="B12" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="45"/>
+      <c r="D12" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E12" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="38"/>
-    </row>
-    <row r="14" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F12" s="45"/>
+      <c r="H12" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="O12" s="26"/>
+    </row>
+    <row r="13" spans="1:23" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="29"/>
+      <c r="J13" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="K13" s="29"/>
+      <c r="L13" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="M13" s="29"/>
+      <c r="N13" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="O13" s="29"/>
+    </row>
+    <row r="14" spans="1:23" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="35"/>
+      <c r="D14" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="H14" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="M14" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="N14" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="O14" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="15" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32"/>
+      <c r="A15" s="5">
+        <v>1</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="H15" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J15" s="24"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="25"/>
     </row>
     <row r="16" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>1</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-    </row>
-    <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="H16" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="24"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="25"/>
+    </row>
+    <row r="17" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>2</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="H17" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17" s="24"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="25"/>
+    </row>
+    <row r="18" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>4</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
+      <c r="H18" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" s="24"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="25"/>
+    </row>
+    <row r="19" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>5</v>
+      </c>
+      <c r="B19" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23"/>
-    </row>
-    <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>3</v>
-      </c>
-      <c r="B18" s="24" t="s">
+      <c r="C19" s="33"/>
+      <c r="D19" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-    </row>
-    <row r="19" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-    </row>
-    <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="H19" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+    </row>
+    <row r="20" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-    </row>
-    <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+    </row>
+    <row r="21" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-    </row>
-    <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+    </row>
+    <row r="22" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+    </row>
+    <row r="23" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="D15:F15"/>
+  <mergeCells count="35">
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D20:F20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D18:F18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="H11:O11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:O12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1892,8 +2539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70A498F-C9BA-4F4A-85D4-1CD05F41A67B}">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,46 +2567,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="D1" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="D2" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="33"/>
+      <c r="E3" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="40"/>
       <c r="G3" s="3"/>
       <c r="I3" s="3"/>
       <c r="K3" s="3"/>
@@ -1986,7 +2633,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2024,42 +2671,42 @@
       <c r="D7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="48"/>
     </row>
     <row r="8" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>1</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="16">
         <v>1</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="29"/>
+      <c r="E8" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="16">
         <v>2</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="29"/>
+      <c r="E9" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:23" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
@@ -2069,159 +2716,159 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
+      <c r="B11" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="1:23" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="38"/>
+      <c r="B13" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="45"/>
       <c r="D13" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="38"/>
+      <c r="F13" s="45"/>
     </row>
     <row r="14" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="30" t="s">
+      <c r="C15" s="35"/>
+      <c r="D15" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
     </row>
     <row r="16" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>1</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
+      <c r="B16" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
     </row>
     <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>2</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23"/>
+      <c r="B17" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
     </row>
     <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>3</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
+      <c r="B18" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>4</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
+      <c r="B19" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
     </row>
     <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>5</v>
       </c>
-      <c r="B20" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
+      <c r="B20" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32"/>
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
     </row>
     <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:F12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:F16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="B18:C18"/>
@@ -2241,12 +2888,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006CB1A51B3A996C44B977E632F6DEC33D" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2bd25917a97534041ca7931abd8cbbac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="66b336d3-04c8-489c-ac96-6a14a2b4331d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="173f2ba09421de1668a77200cfb94d82" ns2:_="">
     <xsd:import namespace="66b336d3-04c8-489c-ac96-6a14a2b4331d"/>
@@ -2378,16 +3034,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08D01FAC-C26F-4BC2-8C04-9A91622ABBCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B439C089-9FB7-457D-8B04-4B618FE47EDC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2396,7 +3051,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C5A42DB-190E-47E2-A19E-CF7C61BA992E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2412,12 +3067,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08D01FAC-C26F-4BC2-8C04-9A91622ABBCA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>